<commit_message>
docs: add to feature list
</commit_message>
<xml_diff>
--- a/To Do List.xlsx
+++ b/To Do List.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="22995" windowHeight="9540"/>
+    <workbookView xWindow="480" yWindow="140" windowWidth="23000" windowHeight="9540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
   <si>
     <t>Feature</t>
   </si>
@@ -67,6 +72,9 @@
   </si>
   <si>
     <t>Docs: Look at every table and begin to construct data map.</t>
+  </si>
+  <si>
+    <t>Feat: Dev prod code to refresh games daily</t>
   </si>
 </sst>
 </file>
@@ -406,19 +414,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="73.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="73.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -429,7 +437,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -440,7 +448,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -451,7 +459,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -462,7 +470,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -473,7 +481,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -484,7 +492,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -495,7 +503,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -506,7 +514,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -517,7 +525,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -528,7 +536,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -539,7 +547,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -550,8 +558,24 @@
         <v>3</v>
       </c>
     </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="1">
+        <v>42515</v>
+      </c>
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -561,9 +585,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -573,8 +602,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
remove to-do list from gen_height fix, add to main to do list
</commit_message>
<xml_diff>
--- a/To Do List.xlsx
+++ b/To Do List.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
   <si>
     <t>Feature</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>Feat: Dev prod code to refresh games daily</t>
+  </si>
+  <si>
+    <t>Feat: Merge Height fix logic into main roster scrape code</t>
   </si>
 </sst>
 </file>
@@ -414,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -566,6 +569,17 @@
         <v>42515</v>
       </c>
       <c r="C13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="1">
+        <v>42515</v>
+      </c>
+      <c r="C14" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: expansion of data integrity checks
</commit_message>
<xml_diff>
--- a/To Do List.xlsx
+++ b/To Do List.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
   <si>
     <t>Feature</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>Feat: Merge Height fix logic into main roster scrape code</t>
+  </si>
+  <si>
+    <t>Feat: Remove BOXT and merge code with main table find process. Just apply fix_bs_starts to all tables.</t>
   </si>
 </sst>
 </file>
@@ -417,15 +420,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="73.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="77.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -581,6 +584,17 @@
       </c>
       <c r="C14" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="1">
+        <v>42524</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: added new to dos
</commit_message>
<xml_diff>
--- a/To Do List.xlsx
+++ b/To Do List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="140" windowWidth="23000" windowHeight="9540"/>
+    <workbookView xWindow="480" yWindow="140" windowWidth="22980" windowHeight="12080"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
   <si>
     <t>Feature</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Checks: Do total points in the game table match the the points in basic stats?</t>
   </si>
   <si>
-    <t>Checks: Do total rebounds in the game table match the the points in basic stats?</t>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
@@ -81,6 +78,27 @@
   </si>
   <si>
     <t>Feat: Remove BOXT and merge code with main table find process. Just apply fix_bs_starts to all tables.</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Complete</t>
+  </si>
+  <si>
+    <t>Checks: Do total rebounds in the game table match the the rebounds in basic stats?</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Several errors were found and fixed. </t>
+  </si>
+  <si>
+    <t>Several errors were found and identified as errors in the source data. Choice has been made to trust the indiidual game files and update the game totals tables accordingly where errors are located. Need to Update the game tables for current year issues</t>
+  </si>
+  <si>
+    <t>In progress</t>
   </si>
 </sst>
 </file>
@@ -116,9 +134,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -420,19 +441,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="77.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="56.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -442,8 +464,14 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -453,8 +481,11 @@
       <c r="C2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -462,10 +493,10 @@
         <v>42515</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -473,56 +504,68 @@
         <v>42515</v>
       </c>
       <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="56">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="1">
+        <v>42515</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
+      <c r="B6" s="1">
+        <v>42515</v>
+      </c>
+      <c r="C6" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="1">
-        <v>42515</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="1">
-        <v>42515</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
+      <c r="B7" s="1">
+        <v>42515</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="1">
-        <v>42515</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
+      <c r="B8" s="1">
+        <v>42515</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
         <v>11</v>
-      </c>
-      <c r="B8" s="1">
-        <v>42515</v>
-      </c>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>12</v>
       </c>
       <c r="B9" s="1">
         <v>42515</v>
@@ -531,31 +574,31 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="1">
+        <v>42515</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="1">
-        <v>42515</v>
-      </c>
-      <c r="C10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
+      <c r="B11" s="1">
+        <v>42515</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
         <v>15</v>
-      </c>
-      <c r="B11" s="1">
-        <v>42515</v>
-      </c>
-      <c r="C11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>16</v>
       </c>
       <c r="B12" s="1">
         <v>42515</v>
@@ -564,37 +607,54 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="1">
+        <v>42515</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="1">
-        <v>42515</v>
-      </c>
-      <c r="C13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
+      <c r="B14" s="1">
+        <v>42515</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
         <v>18</v>
-      </c>
-      <c r="B14" s="1">
-        <v>42515</v>
-      </c>
-      <c r="C14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" t="s">
-        <v>19</v>
       </c>
       <c r="B15" s="1">
         <v>42524</v>
       </c>
       <c r="C15" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3">
+      <c r="C19" s="1">
+        <v>42764</v>
+      </c>
+    </row>
+    <row r="20" spans="3:3">
+      <c r="C20" s="1">
+        <f ca="1">TODAY()</f>
+        <v>42549</v>
+      </c>
+    </row>
+    <row r="21" spans="3:3">
+      <c r="C21">
+        <f ca="1">C19-C20</f>
+        <v>215</v>
       </c>
     </row>
   </sheetData>

</xml_diff>